<commit_message>
move old files away. Separate algorithms by their three classes
</commit_message>
<xml_diff>
--- a/old_files/kim's version of driver, creating clusters etc/tests/Test_results.xlsx
+++ b/old_files/kim's version of driver, creating clusters etc/tests/Test_results.xlsx
@@ -501,7 +501,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R709"/>
+  <dimension ref="A1:R720"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A633" ySplit="1"/>
@@ -49315,6 +49315,665 @@
         <v>3</v>
       </c>
     </row>
+    <row r="710">
+      <c r="A710" t="n">
+        <v>100</v>
+      </c>
+      <c r="B710" t="n">
+        <v>5</v>
+      </c>
+      <c r="C710" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D710" t="inlineStr">
+        <is>
+          <t>ba-no-cycle</t>
+        </is>
+      </c>
+      <c r="E710" t="inlineStr">
+        <is>
+          <t>2021-07-07 21:57:08.700503</t>
+        </is>
+      </c>
+      <c r="F710" t="n">
+        <v>1</v>
+      </c>
+      <c r="G710" t="n">
+        <v>0</v>
+      </c>
+      <c r="H710" t="n">
+        <v>0</v>
+      </c>
+      <c r="I710" t="n">
+        <v>0</v>
+      </c>
+      <c r="J710" t="n">
+        <v>5</v>
+      </c>
+      <c r="K710" t="n">
+        <v>5</v>
+      </c>
+      <c r="L710" t="n">
+        <v>5</v>
+      </c>
+      <c r="M710" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N710" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O710" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="n">
+        <v>100</v>
+      </c>
+      <c r="B711" t="n">
+        <v>5</v>
+      </c>
+      <c r="C711" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D711" t="inlineStr">
+        <is>
+          <t>ba-cycle</t>
+        </is>
+      </c>
+      <c r="E711" t="inlineStr">
+        <is>
+          <t>2021-07-07 21:57:10.072471</t>
+        </is>
+      </c>
+      <c r="F711" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G711" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H711" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I711" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J711" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K711" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L711" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M711" t="n">
+        <v>5</v>
+      </c>
+      <c r="N711" t="n">
+        <v>5</v>
+      </c>
+      <c r="O711" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="n">
+        <v>100</v>
+      </c>
+      <c r="B712" t="n">
+        <v>5</v>
+      </c>
+      <c r="C712" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D712" t="inlineStr">
+        <is>
+          <t>er-no-cycle</t>
+        </is>
+      </c>
+      <c r="E712" t="inlineStr">
+        <is>
+          <t>2021-07-07 21:57:11.260660</t>
+        </is>
+      </c>
+      <c r="F712" t="n">
+        <v>13</v>
+      </c>
+      <c r="G712" t="n">
+        <v>5</v>
+      </c>
+      <c r="H712" t="n">
+        <v>5</v>
+      </c>
+      <c r="I712" t="n">
+        <v>5</v>
+      </c>
+      <c r="J712" t="n">
+        <v>7</v>
+      </c>
+      <c r="K712" t="n">
+        <v>7</v>
+      </c>
+      <c r="L712" t="n">
+        <v>7</v>
+      </c>
+      <c r="M712" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N712" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O712" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="n">
+        <v>100</v>
+      </c>
+      <c r="B713" t="n">
+        <v>5</v>
+      </c>
+      <c r="C713" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D713" t="inlineStr">
+        <is>
+          <t>er-cycle</t>
+        </is>
+      </c>
+      <c r="E713" t="inlineStr">
+        <is>
+          <t>2021-07-07 21:57:12.452814</t>
+        </is>
+      </c>
+      <c r="F713" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G713" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H713" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I713" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J713" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K713" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L713" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M713" t="n">
+        <v>7</v>
+      </c>
+      <c r="N713" t="n">
+        <v>7</v>
+      </c>
+      <c r="O713" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="n">
+        <v>100</v>
+      </c>
+      <c r="B714" t="n">
+        <v>5</v>
+      </c>
+      <c r="C714" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D714" t="inlineStr">
+        <is>
+          <t>ws-no-cycle</t>
+        </is>
+      </c>
+      <c r="E714" t="inlineStr">
+        <is>
+          <t>2021-07-07 21:57:13.604779</t>
+        </is>
+      </c>
+      <c r="F714" t="n">
+        <v>5</v>
+      </c>
+      <c r="G714" t="n">
+        <v>-3</v>
+      </c>
+      <c r="H714" t="n">
+        <v>0</v>
+      </c>
+      <c r="I714" t="n">
+        <v>1</v>
+      </c>
+      <c r="J714" t="n">
+        <v>1</v>
+      </c>
+      <c r="K714" t="n">
+        <v>1</v>
+      </c>
+      <c r="L714" t="n">
+        <v>1</v>
+      </c>
+      <c r="M714" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N714" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O714" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="n">
+        <v>100</v>
+      </c>
+      <c r="B715" t="n">
+        <v>5</v>
+      </c>
+      <c r="C715" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D715" t="inlineStr">
+        <is>
+          <t>ws-cycle</t>
+        </is>
+      </c>
+      <c r="E715" t="inlineStr">
+        <is>
+          <t>2021-07-07 21:57:14.776810</t>
+        </is>
+      </c>
+      <c r="F715" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G715" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H715" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I715" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J715" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K715" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L715" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M715" t="n">
+        <v>1</v>
+      </c>
+      <c r="N715" t="n">
+        <v>1</v>
+      </c>
+      <c r="O715" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="n">
+        <v>100</v>
+      </c>
+      <c r="B716" t="n">
+        <v>5</v>
+      </c>
+      <c r="C716" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D716" t="inlineStr">
+        <is>
+          <t>cluster no cycle</t>
+        </is>
+      </c>
+      <c r="E716" t="inlineStr">
+        <is>
+          <t>2021-07-07 21:57:16.084809</t>
+        </is>
+      </c>
+      <c r="F716" t="n">
+        <v>5</v>
+      </c>
+      <c r="G716" t="n">
+        <v>2</v>
+      </c>
+      <c r="H716" t="n">
+        <v>4</v>
+      </c>
+      <c r="I716" t="n">
+        <v>5</v>
+      </c>
+      <c r="J716" t="n">
+        <v>5</v>
+      </c>
+      <c r="K716" t="n">
+        <v>4</v>
+      </c>
+      <c r="L716" t="n">
+        <v>4</v>
+      </c>
+      <c r="M716" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N716" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O716" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="n">
+        <v>100</v>
+      </c>
+      <c r="B717" t="n">
+        <v>5</v>
+      </c>
+      <c r="C717" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D717" t="inlineStr">
+        <is>
+          <t>cluster cycle</t>
+        </is>
+      </c>
+      <c r="E717" t="inlineStr">
+        <is>
+          <t>2021-07-07 21:57:17.268784</t>
+        </is>
+      </c>
+      <c r="F717" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G717" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H717" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I717" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J717" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K717" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L717" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M717" t="n">
+        <v>14</v>
+      </c>
+      <c r="N717" t="n">
+        <v>14</v>
+      </c>
+      <c r="O717" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="n">
+        <v>100</v>
+      </c>
+      <c r="B718" t="n">
+        <v>5</v>
+      </c>
+      <c r="C718" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D718" t="inlineStr">
+        <is>
+          <t>er</t>
+        </is>
+      </c>
+      <c r="E718" t="inlineStr">
+        <is>
+          <t>2021-07-07 22:25:53.530205</t>
+        </is>
+      </c>
+      <c r="F718" t="n">
+        <v>6</v>
+      </c>
+      <c r="G718" t="n">
+        <v>3</v>
+      </c>
+      <c r="H718" t="n">
+        <v>3</v>
+      </c>
+      <c r="I718" t="n">
+        <v>3</v>
+      </c>
+      <c r="J718" t="n">
+        <v>4</v>
+      </c>
+      <c r="K718" t="n">
+        <v>0</v>
+      </c>
+      <c r="L718" t="n">
+        <v>4</v>
+      </c>
+      <c r="M718" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N718" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O718" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="n">
+        <v>100</v>
+      </c>
+      <c r="B719" t="n">
+        <v>5</v>
+      </c>
+      <c r="C719" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D719" t="inlineStr">
+        <is>
+          <t>ws</t>
+        </is>
+      </c>
+      <c r="E719" t="inlineStr">
+        <is>
+          <t>2021-07-07 22:29:56.838401</t>
+        </is>
+      </c>
+      <c r="F719" t="n">
+        <v>18</v>
+      </c>
+      <c r="G719" t="n">
+        <v>15</v>
+      </c>
+      <c r="H719" t="n">
+        <v>15</v>
+      </c>
+      <c r="I719" t="n">
+        <v>15</v>
+      </c>
+      <c r="J719" t="n">
+        <v>17</v>
+      </c>
+      <c r="K719" t="n">
+        <v>17</v>
+      </c>
+      <c r="L719" t="n">
+        <v>17</v>
+      </c>
+      <c r="M719" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N719" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O719" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="n">
+        <v>100</v>
+      </c>
+      <c r="B720" t="n">
+        <v>5</v>
+      </c>
+      <c r="C720" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D720" t="inlineStr">
+        <is>
+          <t>ba</t>
+        </is>
+      </c>
+      <c r="E720" t="inlineStr">
+        <is>
+          <t>2021-07-07 22:31:40.806195</t>
+        </is>
+      </c>
+      <c r="F720" t="n">
+        <v>9</v>
+      </c>
+      <c r="G720" t="n">
+        <v>6</v>
+      </c>
+      <c r="H720" t="n">
+        <v>6</v>
+      </c>
+      <c r="I720" t="n">
+        <v>6</v>
+      </c>
+      <c r="J720" t="n">
+        <v>6</v>
+      </c>
+      <c r="K720" t="n">
+        <v>6</v>
+      </c>
+      <c r="L720" t="n">
+        <v>6</v>
+      </c>
+      <c r="M720" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N720" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O720" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="Q1:Q1048576 R89:R677">
     <cfRule dxfId="1" operator="equal" priority="1" type="cellIs">
@@ -49334,7 +49993,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L710"/>
+  <dimension ref="A1:L721"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A599" ySplit="1"/>
@@ -82032,6 +82691,500 @@
         <v>0.007329300000000316</v>
       </c>
     </row>
+    <row r="711">
+      <c r="A711" t="n">
+        <v>100</v>
+      </c>
+      <c r="B711" t="n">
+        <v>5</v>
+      </c>
+      <c r="C711" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D711" t="inlineStr">
+        <is>
+          <t>ba-no-cycle</t>
+        </is>
+      </c>
+      <c r="E711" t="inlineStr">
+        <is>
+          <t>2021-07-07 21:57:08.700503</t>
+        </is>
+      </c>
+      <c r="F711" t="n">
+        <v>0.0007806000000001312</v>
+      </c>
+      <c r="G711" t="n">
+        <v>4.589999999993211e-05</v>
+      </c>
+      <c r="H711" t="n">
+        <v>0.01034859999999993</v>
+      </c>
+      <c r="I711" t="n">
+        <v>0.06480240000000004</v>
+      </c>
+      <c r="J711" t="n">
+        <v>0.03814990000000007</v>
+      </c>
+      <c r="K711" t="n">
+        <v>0.002122400000000191</v>
+      </c>
+      <c r="L711" t="n">
+        <v>0.00564349999999969</v>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="n">
+        <v>100</v>
+      </c>
+      <c r="B712" t="n">
+        <v>5</v>
+      </c>
+      <c r="C712" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D712" t="inlineStr">
+        <is>
+          <t>ba-cycle</t>
+        </is>
+      </c>
+      <c r="E712" t="inlineStr">
+        <is>
+          <t>2021-07-07 21:57:10.072471</t>
+        </is>
+      </c>
+      <c r="F712" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G712" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H712" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I712" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J712" t="n">
+        <v>0.0356285999999999</v>
+      </c>
+      <c r="K712" t="n">
+        <v>0.002568799999999705</v>
+      </c>
+      <c r="L712" t="n">
+        <v>0.005386599999999575</v>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="n">
+        <v>100</v>
+      </c>
+      <c r="B713" t="n">
+        <v>5</v>
+      </c>
+      <c r="C713" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D713" t="inlineStr">
+        <is>
+          <t>er-no-cycle</t>
+        </is>
+      </c>
+      <c r="E713" t="inlineStr">
+        <is>
+          <t>2021-07-07 21:57:11.260660</t>
+        </is>
+      </c>
+      <c r="F713" t="n">
+        <v>0.0004996000000003775</v>
+      </c>
+      <c r="G713" t="n">
+        <v>6.180000000011177e-05</v>
+      </c>
+      <c r="H713" t="n">
+        <v>0.0007615000000003036</v>
+      </c>
+      <c r="I713" t="n">
+        <v>0.03180160000000054</v>
+      </c>
+      <c r="J713" t="n">
+        <v>0.03520939999999939</v>
+      </c>
+      <c r="K713" t="n">
+        <v>0.001506000000000007</v>
+      </c>
+      <c r="L713" t="n">
+        <v>0.004215000000000302</v>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="n">
+        <v>100</v>
+      </c>
+      <c r="B714" t="n">
+        <v>5</v>
+      </c>
+      <c r="C714" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D714" t="inlineStr">
+        <is>
+          <t>er-cycle</t>
+        </is>
+      </c>
+      <c r="E714" t="inlineStr">
+        <is>
+          <t>2021-07-07 21:57:12.452814</t>
+        </is>
+      </c>
+      <c r="F714" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G714" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H714" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I714" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J714" t="n">
+        <v>0.03518810000000006</v>
+      </c>
+      <c r="K714" t="n">
+        <v>0.001177300000000159</v>
+      </c>
+      <c r="L714" t="n">
+        <v>0.003954600000000141</v>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="n">
+        <v>100</v>
+      </c>
+      <c r="B715" t="n">
+        <v>5</v>
+      </c>
+      <c r="C715" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D715" t="inlineStr">
+        <is>
+          <t>ws-no-cycle</t>
+        </is>
+      </c>
+      <c r="E715" t="inlineStr">
+        <is>
+          <t>2021-07-07 21:57:13.604779</t>
+        </is>
+      </c>
+      <c r="F715" t="n">
+        <v>0.0009300999999997117</v>
+      </c>
+      <c r="G715" t="n">
+        <v>4.490000000068051e-05</v>
+      </c>
+      <c r="H715" t="n">
+        <v>0.001740199999998637</v>
+      </c>
+      <c r="I715" t="n">
+        <v>0.03593919999999962</v>
+      </c>
+      <c r="J715" t="n">
+        <v>0.0347767000000001</v>
+      </c>
+      <c r="K715" t="n">
+        <v>0.002935799999999489</v>
+      </c>
+      <c r="L715" t="n">
+        <v>0.004860799999999443</v>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="n">
+        <v>100</v>
+      </c>
+      <c r="B716" t="n">
+        <v>5</v>
+      </c>
+      <c r="C716" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D716" t="inlineStr">
+        <is>
+          <t>ws-cycle</t>
+        </is>
+      </c>
+      <c r="E716" t="inlineStr">
+        <is>
+          <t>2021-07-07 21:57:14.776810</t>
+        </is>
+      </c>
+      <c r="F716" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G716" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H716" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I716" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J716" t="n">
+        <v>0.03404320000000105</v>
+      </c>
+      <c r="K716" t="n">
+        <v>0.00248810000000077</v>
+      </c>
+      <c r="L716" t="n">
+        <v>0.004376300000000555</v>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="n">
+        <v>100</v>
+      </c>
+      <c r="B717" t="n">
+        <v>5</v>
+      </c>
+      <c r="C717" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D717" t="inlineStr">
+        <is>
+          <t>cluster no cycle</t>
+        </is>
+      </c>
+      <c r="E717" t="inlineStr">
+        <is>
+          <t>2021-07-07 21:57:16.084809</t>
+        </is>
+      </c>
+      <c r="F717" t="n">
+        <v>0.001307899999998696</v>
+      </c>
+      <c r="G717" t="n">
+        <v>6.310000000020466e-05</v>
+      </c>
+      <c r="H717" t="n">
+        <v>0.1136543999999997</v>
+      </c>
+      <c r="I717" t="n">
+        <v>0.03617579999999876</v>
+      </c>
+      <c r="J717" t="n">
+        <v>0.03291789999999928</v>
+      </c>
+      <c r="K717" t="n">
+        <v>0.001879999999999882</v>
+      </c>
+      <c r="L717" t="n">
+        <v>0.007716600000000184</v>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="n">
+        <v>100</v>
+      </c>
+      <c r="B718" t="n">
+        <v>5</v>
+      </c>
+      <c r="C718" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D718" t="inlineStr">
+        <is>
+          <t>cluster cycle</t>
+        </is>
+      </c>
+      <c r="E718" t="inlineStr">
+        <is>
+          <t>2021-07-07 21:57:17.268784</t>
+        </is>
+      </c>
+      <c r="F718" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G718" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H718" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I718" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J718" t="n">
+        <v>0.03537269999999992</v>
+      </c>
+      <c r="K718" t="n">
+        <v>0.003301100000001611</v>
+      </c>
+      <c r="L718" t="n">
+        <v>0.008220299999999625</v>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="n">
+        <v>100</v>
+      </c>
+      <c r="B719" t="n">
+        <v>5</v>
+      </c>
+      <c r="C719" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D719" t="inlineStr">
+        <is>
+          <t>er</t>
+        </is>
+      </c>
+      <c r="E719" t="inlineStr">
+        <is>
+          <t>2021-07-07 22:25:53.530205</t>
+        </is>
+      </c>
+      <c r="F719" t="n">
+        <v>0.0006656999999998803</v>
+      </c>
+      <c r="G719" t="n">
+        <v>9.639999999988547e-05</v>
+      </c>
+      <c r="H719" t="n">
+        <v>0.001335700000000051</v>
+      </c>
+      <c r="I719" t="n">
+        <v>0.05504299999999995</v>
+      </c>
+      <c r="J719" t="n">
+        <v>0.05082720000000007</v>
+      </c>
+      <c r="K719" t="n">
+        <v>0.0032582000000001</v>
+      </c>
+      <c r="L719" t="n">
+        <v>0.008643699999999921</v>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="n">
+        <v>100</v>
+      </c>
+      <c r="B720" t="n">
+        <v>5</v>
+      </c>
+      <c r="C720" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D720" t="inlineStr">
+        <is>
+          <t>ws</t>
+        </is>
+      </c>
+      <c r="E720" t="inlineStr">
+        <is>
+          <t>2021-07-07 22:29:56.838401</t>
+        </is>
+      </c>
+      <c r="F720" t="n">
+        <v>0.0007159999999999389</v>
+      </c>
+      <c r="G720" t="n">
+        <v>6.680000000014452e-05</v>
+      </c>
+      <c r="H720" t="n">
+        <v>0.004442199999999952</v>
+      </c>
+      <c r="I720" t="n">
+        <v>0.05318109999999998</v>
+      </c>
+      <c r="J720" t="n">
+        <v>0.06027199999999988</v>
+      </c>
+      <c r="K720" t="n">
+        <v>0.003525299999999953</v>
+      </c>
+      <c r="L720" t="n">
+        <v>0.01144409999999985</v>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="n">
+        <v>100</v>
+      </c>
+      <c r="B721" t="n">
+        <v>5</v>
+      </c>
+      <c r="C721" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D721" t="inlineStr">
+        <is>
+          <t>ba</t>
+        </is>
+      </c>
+      <c r="E721" t="inlineStr">
+        <is>
+          <t>2021-07-07 22:31:40.806195</t>
+        </is>
+      </c>
+      <c r="F721" t="n">
+        <v>0.0007654000000001382</v>
+      </c>
+      <c r="G721" t="n">
+        <v>7.099999999993223e-05</v>
+      </c>
+      <c r="H721" t="n">
+        <v>0.003318500000000002</v>
+      </c>
+      <c r="I721" t="n">
+        <v>0.0458464999999999</v>
+      </c>
+      <c r="J721" t="n">
+        <v>0.05280600000000013</v>
+      </c>
+      <c r="K721" t="n">
+        <v>0.002782000000000062</v>
+      </c>
+      <c r="L721" t="n">
+        <v>0.009597299999999809</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>